<commit_message>
add fr jurisdiction, snomed parameters, ... b874081cbff5bf4e1f657ae782a49d62b89dc1e7
</commit_message>
<xml_diff>
--- a/nr-review/ig/CodeSystem-fr-additional-action-relationship-type.xlsx
+++ b/nr-review/ig/CodeSystem-fr-additional-action-relationship-type.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-11T12:24:54+00:00</t>
+    <t>2025-07-11T12:29:53+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Jurisdiction</t>
   </si>
   <si>
-    <t/>
+    <t>FRANCE</t>
   </si>
   <si>
     <t>Description</t>

</xml_diff>

<commit_message>
suppression exemple marsilid zomigoro et enlever code EXCL du CS FrAdditionalActionRelationshipType f789da679037d12e0deaf8ffa50ac30a43c4e3dd
</commit_message>
<xml_diff>
--- a/nr-review/ig/CodeSystem-fr-additional-action-relationship-type.xlsx
+++ b/nr-review/ig/CodeSystem-fr-additional-action-relationship-type.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-18T14:33:50+00:00</t>
+    <t>2025-07-21T08:56:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -136,12 +136,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>EXCL</t>
-  </si>
-  <si>
-    <t>Si l'action est réalisée, l'action reliée ne doit pas être effectuée.</t>
   </si>
   <si>
     <t>ALT</t>
@@ -458,7 +452,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -490,18 +484,6 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>